<commit_message>
CodeBooks testing. Emails are impported
</commit_message>
<xml_diff>
--- a/Refuntations_App/wwwroot/IMPORT - INTERNI DOBAVLJACI - EMAIL ADRESE.xlsx
+++ b/Refuntations_App/wwwroot/IMPORT - INTERNI DOBAVLJACI - EMAIL ADRESE.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dste848075\Desktop\Refundacije\Refuntations_App\wwwroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dste848075\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7770"/>
   </bookViews>
   <sheets>
-    <sheet name="IMPORT" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,39 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Šifra dobavljača</t>
+    <t>ŠIFRA DOBAVLJAČA SAP</t>
   </si>
   <si>
-    <t>SAP šifra dobavljača</t>
-  </si>
-  <si>
-    <t>Naziv dobavljača</t>
-  </si>
-  <si>
-    <t>Email dobavljača</t>
+    <t>EMAIL ADRESA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -80,16 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -372,36 +350,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="88.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>